<commit_message>
I updated the test files for the program; I update the file to save the data after generating letters. I added EXCEL_FILE_PATH ,SKYFEND_BUSINESS_PATH,PROCESSED_EXCEL_FILE_PATH to the main.py, update related files. ied:   tests/test_identify_cooperation_points.py
</commit_message>
<xml_diff>
--- a/data/raw/test_to_read_website.xlsx
+++ b/data/raw/test_to_read_website.xlsx
@@ -1,104 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junluo/Documents/Send_Developing_Letters/data/raw/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEB2BCA-2480-BC40-94AF-47D736ABF482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{FB599239-2A21-FA4A-AE58-266D65A4B14C}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.google.com
-</t>
-  </si>
-  <si>
-    <t>google</t>
-  </si>
-  <si>
-    <t>recipient_email</t>
-  </si>
-  <si>
-    <t>testing1@gmail.com</t>
-  </si>
-  <si>
-    <t>contact person</t>
-  </si>
-  <si>
-    <t>John Chen</t>
-  </si>
-  <si>
-    <t>Process</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="16"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="16"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="16"/>
-      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="16"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -161,50 +104,140 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -524,198 +557,294 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8A7B48-6931-EC49-B4F2-907189FB2DBB}">
-  <dimension ref="A1:E61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="22"/>
   <cols>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="207" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="6"/>
-      <c r="C44" s="7"/>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="6"/>
-      <c r="C45" s="7"/>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="6"/>
-      <c r="C47" s="8"/>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Process</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Company</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Website</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>recipient_email</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>contact person</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="207" customHeight="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>google</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://www.google.com
+</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>testing1@gmail.com</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>John Chen</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" s="2" t="n"/>
+      <c r="D3" s="2" t="n"/>
+    </row>
+    <row r="32">
+      <c r="B32" s="6" t="n"/>
+      <c r="C32" s="6" t="n"/>
+    </row>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42">
+      <c r="B42" s="6" t="n"/>
+      <c r="C42" s="6" t="n"/>
+    </row>
+    <row r="43"/>
+    <row r="44">
+      <c r="B44" s="6" t="n"/>
+      <c r="C44" s="7" t="n"/>
+    </row>
+    <row r="45">
+      <c r="C45" s="9" t="n"/>
+    </row>
+    <row r="46">
+      <c r="B46" s="6" t="n"/>
+      <c r="C46" s="8" t="n"/>
+    </row>
+    <row r="47">
+      <c r="C47" s="10" t="n"/>
+    </row>
+    <row r="48">
+      <c r="B48" s="11" t="n"/>
+      <c r="C48" s="11" t="n"/>
+    </row>
+    <row r="49">
+      <c r="B49" s="12" t="n"/>
+      <c r="C49" s="12" t="n"/>
+    </row>
+    <row r="50">
+      <c r="B50" s="11" t="n"/>
+      <c r="C50" s="11" t="n"/>
+    </row>
+    <row r="51">
+      <c r="B51" s="13" t="n"/>
+      <c r="C51" s="13" t="n"/>
+    </row>
+    <row r="52">
+      <c r="B52" s="13" t="n"/>
+      <c r="C52" s="13" t="n"/>
+    </row>
+    <row r="53">
+      <c r="B53" s="13" t="n"/>
+      <c r="C53" s="13" t="n"/>
+    </row>
+    <row r="54">
+      <c r="B54" s="13" t="n"/>
+      <c r="C54" s="13" t="n"/>
+    </row>
+    <row r="55">
+      <c r="B55" s="13" t="n"/>
+      <c r="C55" s="13" t="n"/>
+    </row>
+    <row r="56">
+      <c r="B56" s="13" t="n"/>
+      <c r="C56" s="13" t="n"/>
+    </row>
+    <row r="57">
+      <c r="B57" s="13" t="n"/>
+      <c r="C57" s="13" t="n"/>
+    </row>
+    <row r="58">
+      <c r="B58" s="13" t="n"/>
+      <c r="C58" s="13" t="n"/>
+    </row>
+    <row r="59">
+      <c r="B59" s="12" t="n"/>
+      <c r="C59" s="12" t="n"/>
+    </row>
+    <row r="60">
+      <c r="B60" s="11" t="n"/>
+      <c r="C60" s="11" t="n"/>
+    </row>
+    <row r="61">
+      <c r="B61" s="12" t="n"/>
+      <c r="C61" s="12" t="n"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025/03/15 10:12</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>google</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>https://www.google.com</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Google is a technology company that specializes in internet-related services and products, including search engines, online advertising technologies, cloud computing, software, and hardware. Its primary activity is organizing the world's information and making it universally accessible and useful through its search engine and various other digital services.</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Dear John Chen,&lt;/p&gt;
+&lt;p&gt;I hope this message finds you well. My name is Jimmy, and I am the Overseas Sales Manager at &lt;strong&gt;Skyfend&lt;/strong&gt;, a subsidiary of Autel. We have been closely following Google’s remarkable advancements and believe there is significant potential for collaboration between our companies.&lt;/p&gt;
+&lt;p&gt;Skyfend has established a strong global presence, exporting advanced counter-drone devices to partners across Africa, Europe, and America. Our solutions, such as the &lt;strong&gt;Tracer&lt;/strong&gt; and &lt;strong&gt;Defender&lt;/strong&gt; systems, are designed to address FPV drone threats and ensure the security of commercial drones like DJI, Autel, and Parrot.&lt;/p&gt;
+&lt;p&gt;I would like to propose a strategic partnership to explore the following cooperation opportunities:&lt;/p&gt;
+&lt;ul&gt;
+  &lt;li&gt;&lt;strong&gt;AI/ML-Enhanced Drone Threat Detection &amp; Prediction:&lt;/strong&gt; Integrating Google’s AI/ML tools with Skyfend’s detection systems to improve accuracy and predict intrusion patterns.&lt;/li&gt;
+  &lt;li&gt;&lt;strong&gt;Cloud-Based Command &amp; Control Infrastructure:&lt;/strong&gt; Hosting Skyfend’s Guider C2 software on Google Cloud for scalable, real-time analytics.&lt;/li&gt;
+  &lt;li&gt;&lt;strong&gt;Secure Airspace Solutions for Google Wing Drone Deliveries:&lt;/strong&gt; Protecting delivery drones with Skyfend’s portable jammers and spoofers.&lt;/li&gt;
+  &lt;li&gt;&lt;strong&gt;Geospatial Threat Mapping with Google Earth/Maps:&lt;/strong&gt; Visualizing real-time drone threats using Google’s geospatial APIs.&lt;/li&gt;
+  &lt;li&gt;&lt;strong&gt;IoT-Enabled Security Ecosystems:&lt;/strong&gt; Combining Skyfend’s detectors with Google Nest or Android platforms for smart perimeter security.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;I have attached a product brochure for your reference. I would be delighted to schedule a video meeting or call to discuss these opportunities further. Please let me know your availability.&lt;/p&gt;
+&lt;p&gt;Looking forward to your response.&lt;/p&gt;
+&lt;p&gt;Best regards,&lt;br&gt;Jimmy&lt;br&gt;Overseas Sales Manager&lt;br&gt;Skyfend&lt;/p&gt;</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>testing1@gmail.com</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>John Chen</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025/03/15 10:16</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>google</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>https://www.google.com</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Google is a technology company that specializes in internet-related services and products, including search engines, online advertising, cloud computing, software, and hardware. Its primary activity is organizing the world's information and making it universally accessible and useful through its search engine and various other digital services.</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>&lt;p&gt;Dear John Chen,&lt;/p&gt;
+&lt;p&gt;I hope this message finds you well. We at &lt;strong&gt;Skyfend&lt;/strong&gt;, a subsidiary of Autel, have been closely following Google’s remarkable advancements in technology and innovation. As the Overseas Sales Manager, I am excited to explore potential collaboration opportunities between our companies.&lt;/p&gt;
+&lt;p&gt;Skyfend has established a strong global presence, exporting advanced counter-drone devices to partners across Africa, Europe, and America. Our expertise lies in addressing FPV drone threats and managing commercial drones from leading brands like DJI, Autel, and Parrot. We believe that combining our domain expertise with Google’s technological prowess could unlock significant synergies.&lt;/p&gt;
+&lt;p&gt;Here are a few areas where we see potential for collaboration:&lt;/p&gt;
+&lt;ul&gt;
+  &lt;li&gt;&lt;strong&gt;AI/ML Integration:&lt;/strong&gt; Leveraging Google’s TensorFlow or Vertex AI to enhance Skyfend’s detection algorithms, reducing false positives and improving real-time threat classification.&lt;/li&gt;
+  &lt;li&gt;&lt;strong&gt;Google Cloud for Data Analytics:&lt;/strong&gt; Utilizing BigQuery and Looker for predictive analytics and threat pattern recognition from Skyfend’s sensor data.&lt;/li&gt;
+  &lt;li&gt;&lt;strong&gt;Airspace Security with Google Wing:&lt;/strong&gt; Integrating Skyfend’s C-UAS solutions with Project Wing to create safe corridors for delivery drones.&lt;/li&gt;
+  &lt;li&gt;&lt;strong&gt;Android/Pixel Integration:&lt;/strong&gt; Embedding Google’s Android OS or Titan M2 chips into Skyfend’s portable devices for enhanced user interfaces and secure communication.&lt;/li&gt;
+  &lt;li&gt;&lt;strong&gt;Geolocation Precision:&lt;/strong&gt; Enhancing Skyfend’s spoofing/jamming accuracy using Google Maps/Earth APIs for real-time terrain and 3D mapping data.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;I would love to discuss these opportunities further. Could we schedule a video meeting or call at your convenience? I have also attached a product brochure for your reference.&lt;/p&gt;
+&lt;p&gt;Looking forward to your response.&lt;/p&gt;
+&lt;p&gt;Best regards,&lt;br&gt;
+Jimmy&lt;br&gt;
+Overseas Sales Manager&lt;br&gt;
+Skyfend&lt;/p&gt;</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>testing1@gmail.com</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>John Chen</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C50:C59"/>
     <mergeCell ref="B32:B41"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C48:C49"/>
     <mergeCell ref="C32:C41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C42:C43"/>
     <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="B48:B49"/>
     <mergeCell ref="B50:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C50:C59"/>
-    <mergeCell ref="C60:C61"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{5A7F6C68-FA6A-F145-8D85-F486EAE05040}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{99EF6B48-6A47-DB42-8326-4495A6D7E893}"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
I added the function to insert the image in the email body( attach images inline)
</commit_message>
<xml_diff>
--- a/data/raw/test_to_read_website.xlsx
+++ b/data/raw/test_to_read_website.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junluo/Documents/Send_Developing_Letters/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B86CDB-FA47-3D4D-BD76-E9E294772360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0BDA42-34D0-B948-8F70-1A9634CB12D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -227,29 +227,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -588,7 +585,7 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
@@ -615,24 +612,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="207" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="207" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="53" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -642,7 +639,7 @@
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>23</v>
       </c>
       <c r="E3" t="s">
@@ -656,10 +653,10 @@
       <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E4" t="s">
@@ -673,10 +670,10 @@
       <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E5" t="s">
@@ -684,124 +681,124 @@
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="5"/>
-      <c r="C45" s="10"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="8"/>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="6"/>
-      <c r="C46" s="11"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="9"/>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="5"/>
-      <c r="C47" s="8"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="4"/>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="6"/>
-      <c r="C48" s="9"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="5"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
@@ -851,6 +848,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C51:C60"/>
+    <mergeCell ref="B51:B60"/>
     <mergeCell ref="B33:B42"/>
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="B43:B44"/>
@@ -859,12 +862,6 @@
     <mergeCell ref="C45:C46"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C51:C60"/>
-    <mergeCell ref="B51:B60"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -874,6 +871,7 @@
     <hyperlink ref="C5" r:id="rId5" xr:uid="{BFCC66B6-B16B-684E-B781-B7F8AC90CB22}"/>
     <hyperlink ref="C3" r:id="rId6" xr:uid="{A0040A3A-3592-694D-81AB-C2B85BF07B60}"/>
     <hyperlink ref="D3" r:id="rId7" xr:uid="{5B11A7A8-2376-1341-BD32-0CE8B3CD6CE8}"/>
+    <hyperlink ref="D5" r:id="rId8" xr:uid="{853DB241-2C4A-FE45-883D-00E514BA4777}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
I added a function that attach the files to the email that will save in google draft. the instructions I used are "1. first, I need to create a [main4.py](http://main4.py) to achieve the function as I wanna keep the function of [main3.py](http://main2.py) and [main2.py](http://main2.py) 2. I need to prepare files that need to be put in the attachment; the address is :/Users/junluo/Documents/Send_Developing_Letters/data/raw/files/1.Product brochure of Skyfend.pdf 3. the program only attaches files when saving the email draft in google account, doesn't save the file to other places. 4. which files that I need to update codes to achieve the function I need? 5. show me the complete codes for these files"
</commit_message>
<xml_diff>
--- a/data/raw/test_to_read_website.xlsx
+++ b/data/raw/test_to_read_website.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junluo/Documents/Send_Developing_Letters/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0BDA42-34D0-B948-8F70-1A9634CB12D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0514850-79BE-2D4A-973D-0BF05899C25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Process</t>
   </si>
@@ -116,16 +116,35 @@
     <t>Alexander Wulf</t>
   </si>
   <si>
-    <t>Florian Kleinig</t>
-  </si>
-  <si>
-    <t>florian.kleinig@droniq.de</t>
-  </si>
-  <si>
     <t>testing22@gmail.com</t>
   </si>
   <si>
     <t>Jack</t>
+  </si>
+  <si>
+    <t>Jack  Kleinig</t>
+  </si>
+  <si>
+    <t>jack.kleinig@droniq.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drone Volt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.dronevolt.com/
+</t>
+  </si>
+  <si>
+    <t>Olivier Gualdoni</t>
+  </si>
+  <si>
+    <t>olivier@dronevolt.com</t>
+  </si>
+  <si>
+    <t>Stefano Valentini</t>
+  </si>
+  <si>
+    <t>stefano.valentini@dronevolt.com</t>
   </si>
 </sst>
 </file>
@@ -585,14 +604,14 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="4" max="4" width="22.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -640,10 +659,10 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -674,10 +693,44 @@
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
@@ -872,6 +925,10 @@
     <hyperlink ref="C3" r:id="rId6" xr:uid="{A0040A3A-3592-694D-81AB-C2B85BF07B60}"/>
     <hyperlink ref="D3" r:id="rId7" xr:uid="{5B11A7A8-2376-1341-BD32-0CE8B3CD6CE8}"/>
     <hyperlink ref="D5" r:id="rId8" xr:uid="{853DB241-2C4A-FE45-883D-00E514BA4777}"/>
+    <hyperlink ref="C6" r:id="rId9" xr:uid="{87BFAC37-3FC4-6A40-8AFF-51652BDC583D}"/>
+    <hyperlink ref="D6" r:id="rId10" xr:uid="{EEE3F8A9-5CFC-D64A-98F3-CF0DB0973488}"/>
+    <hyperlink ref="D7" r:id="rId11" xr:uid="{EB1C5524-5EFE-A144-910A-BCEDF4BC1862}"/>
+    <hyperlink ref="C7" r:id="rId12" xr:uid="{D45BA856-1165-0D47-85AA-562ABDB2DD74}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
I deleted the virtual environment I created before by using the one poetry creates for me. I update pyproject.txt and poetry.lock.
</commit_message>
<xml_diff>
--- a/data/raw/test_to_read_website.xlsx
+++ b/data/raw/test_to_read_website.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junluo/Documents/Send_Developing_Letters/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0514850-79BE-2D4A-973D-0BF05899C25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F8999F-11A1-5340-A10E-C8DDB59D6E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
   <si>
     <t>Process</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>stefano.valentini@dronevolt.com</t>
+  </si>
+  <si>
+    <t>jimm123@dronevolt.com</t>
+  </si>
+  <si>
+    <t>Jimmy</t>
   </si>
 </sst>
 </file>
@@ -249,23 +255,23 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -604,7 +610,7 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
@@ -733,125 +739,142 @@
         <v>29</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="2"/>
-      <c r="C45" s="8"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="9"/>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="3"/>
-      <c r="C46" s="9"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="10"/>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="2"/>
-      <c r="C47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="7"/>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="3"/>
-      <c r="C48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="8"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B61" s="6"/>
-      <c r="C61" s="6"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
@@ -901,12 +924,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C51:C60"/>
-    <mergeCell ref="B51:B60"/>
     <mergeCell ref="B33:B42"/>
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="B43:B44"/>
@@ -915,6 +932,12 @@
     <mergeCell ref="C45:C46"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C51:C60"/>
+    <mergeCell ref="B51:B60"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -929,6 +952,8 @@
     <hyperlink ref="D6" r:id="rId10" xr:uid="{EEE3F8A9-5CFC-D64A-98F3-CF0DB0973488}"/>
     <hyperlink ref="D7" r:id="rId11" xr:uid="{EB1C5524-5EFE-A144-910A-BCEDF4BC1862}"/>
     <hyperlink ref="C7" r:id="rId12" xr:uid="{D45BA856-1165-0D47-85AA-562ABDB2DD74}"/>
+    <hyperlink ref="C8" r:id="rId13" xr:uid="{3AA63318-B004-BF4C-BFA8-7592A015A849}"/>
+    <hyperlink ref="D8" r:id="rId14" xr:uid="{A70CFB6E-9DC6-8244-B38C-ABDC590428A9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
when loading the client data, I set if the value of the "Process" column is "yes", then process on; if it is not "yes", skip it.
</commit_message>
<xml_diff>
--- a/data/raw/test_to_read_website.xlsx
+++ b/data/raw/test_to_read_website.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junluo/Documents/Send_Developing_Letters/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F8999F-11A1-5340-A10E-C8DDB59D6E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A2DEA6-99C4-784D-88F4-DB0978EEBF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>Process</t>
   </si>
@@ -151,6 +151,22 @@
   </si>
   <si>
     <t>Jimmy</t>
+  </si>
+  <si>
+    <t>Center for Service of National Police Units of Ukraine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mvs.gov.ua/en/contacts/national-police-ukraine
+</t>
+  </si>
+  <si>
+    <t>anketa.bezvisty@mvs.gov.ua</t>
+  </si>
+  <si>
+    <t>Anketa Bezvisty</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -610,14 +626,14 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="22.125" customWidth="1"/>
+    <col min="3" max="3" width="31.875" customWidth="1"/>
+    <col min="4" max="4" width="26.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -749,12 +765,33 @@
       <c r="C8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>31</v>
       </c>
       <c r="E8" t="s">
         <v>32</v>
       </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" s="4"/>
@@ -952,8 +989,10 @@
     <hyperlink ref="D6" r:id="rId10" xr:uid="{EEE3F8A9-5CFC-D64A-98F3-CF0DB0973488}"/>
     <hyperlink ref="D7" r:id="rId11" xr:uid="{EB1C5524-5EFE-A144-910A-BCEDF4BC1862}"/>
     <hyperlink ref="C7" r:id="rId12" xr:uid="{D45BA856-1165-0D47-85AA-562ABDB2DD74}"/>
-    <hyperlink ref="C8" r:id="rId13" xr:uid="{3AA63318-B004-BF4C-BFA8-7592A015A849}"/>
-    <hyperlink ref="D8" r:id="rId14" xr:uid="{A70CFB6E-9DC6-8244-B38C-ABDC590428A9}"/>
+    <hyperlink ref="D8" r:id="rId13" xr:uid="{A70CFB6E-9DC6-8244-B38C-ABDC590428A9}"/>
+    <hyperlink ref="C8" r:id="rId14" xr:uid="{3AA63318-B004-BF4C-BFA8-7592A015A849}"/>
+    <hyperlink ref="D9" r:id="rId15" xr:uid="{DE278980-CCB7-0443-AECF-54B6E565E304}"/>
+    <hyperlink ref="C9" r:id="rId16" xr:uid="{78C49266-BAB8-F641-BF34-A6A36A3C833E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>